<commit_message>
organization and best practice
</commit_message>
<xml_diff>
--- a/fichiers_jeux_de_donnees/Excel Chart Customization.xlsx
+++ b/fichiers_jeux_de_donnees/Excel Chart Customization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\logiciels_et_projets\excel_data_viz\fichiers_jeux_de_donnees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430E032A-E547-4140-8B43-7706FBA649A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFF7503-A267-45E9-B944-0E763008166E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3FD3964C-8F62-4B74-B4B4-34AD1ABBA03A}"/>
   </bookViews>
@@ -391,6 +391,22 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="901782720"/>
+        <c:axId val="901773600"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -406,20 +422,31 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="bg2"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Data!$A$2:$A$13</c:f>
@@ -509,6 +536,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8FC6-4A34-AA5C-4C7F640F6893}"/>
@@ -523,10 +551,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="901782720"/>
         <c:axId val="901773600"/>
-      </c:barChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="901782720"/>
         <c:scaling>
@@ -744,6 +773,45 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4171,7 +4239,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>